<commit_message>
Two more ManagePage tests
ChangePasswordwithInvalidNewPassword,
ChangePasswordwithoutConfirmedNewPassword
</commit_message>
<xml_diff>
--- a/Blog-Skeleton/Blog.NUnit.Tests/TestData/UserData.xlsx
+++ b/Blog-Skeleton/Blog.NUnit.Tests/TestData/UserData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="8505" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="9105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="LoginUser" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Key</t>
   </si>
@@ -47,6 +47,18 @@
   </si>
   <si>
     <t>ChangePasswordwithInvalidCurrentPassword</t>
+  </si>
+  <si>
+    <t>ChangePasswordwithInvalidNewPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ChangePasswordwithoutConfirmedNewPassword</t>
+  </si>
+  <si>
+    <t>pass</t>
   </si>
 </sst>
 </file>
@@ -402,12 +414,12 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -461,14 +473,52 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
       <c r="H4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Manoela Failing Registration with the same user
Server Error appears so test should fail.
</commit_message>
<xml_diff>
--- a/Blog-Skeleton/Blog.NUnit.Tests/TestData/UserData.xlsx
+++ b/Blog-Skeleton/Blog.NUnit.Tests/TestData/UserData.xlsx
@@ -134,7 +134,7 @@
     <t>RegisterWithTheSameEmail</t>
   </si>
   <si>
-    <t>UserId not found.</t>
+    <t>The Email address is already registered.</t>
   </si>
 </sst>
 </file>
@@ -608,7 +608,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added CMS tests with logged user
Added CMS tests with logged user;
Note - one of the test does not pass. Explained as comment on the said
test.
Added a new worksheet in the UserData.xlsx;
Verified if added test are logged in the Log.txt;
</commit_message>
<xml_diff>
--- a/Blog-Skeleton/Blog.NUnit.Tests/TestData/UserData.xlsx
+++ b/Blog-Skeleton/Blog.NUnit.Tests/TestData/UserData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="9105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginUser" sheetId="1" r:id="rId1"/>
-    <sheet name="RegisterUser" sheetId="2" r:id="rId2"/>
+    <sheet name="Articles" sheetId="3" r:id="rId2"/>
+    <sheet name="RegisterUser" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
   <si>
     <t>Key</t>
   </si>
@@ -135,6 +136,108 @@
   </si>
   <si>
     <t>The Email address is already registered.</t>
+  </si>
+  <si>
+    <t>CreateNewArticle</t>
+  </si>
+  <si>
+    <t>abv@abv.bg</t>
+  </si>
+  <si>
+    <t>TargetForEdit</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>ArticleErrorMessage</t>
+  </si>
+  <si>
+    <t>AdditionalErrorMessage</t>
+  </si>
+  <si>
+    <t>CreateNewArticleWithValidData</t>
+  </si>
+  <si>
+    <t>TestArticle</t>
+  </si>
+  <si>
+    <t>Dear Reader, this is an article for testing purposes.</t>
+  </si>
+  <si>
+    <t>EditExistingArticle</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>Dear Reader! This is an article for testing purposes!</t>
+  </si>
+  <si>
+    <t>DeleteExistingArticle</t>
+  </si>
+  <si>
+    <t>CreateArticleWithoutTitle</t>
+  </si>
+  <si>
+    <t>The title is empty.</t>
+  </si>
+  <si>
+    <t>The Title field is required.</t>
+  </si>
+  <si>
+    <t>CreateArticleWithoutContent</t>
+  </si>
+  <si>
+    <t>InvalidArticleContent</t>
+  </si>
+  <si>
+    <t>The Content field is required.</t>
+  </si>
+  <si>
+    <t>CreateArticleWithoutTitleAndContent</t>
+  </si>
+  <si>
+    <t>CreateArticleWithLongTitle</t>
+  </si>
+  <si>
+    <t>This article's title is longer than fifty (50) symbols.</t>
+  </si>
+  <si>
+    <t>The title is too long.</t>
+  </si>
+  <si>
+    <t>The field Title must be a string with a maximum length of 50.</t>
+  </si>
+  <si>
+    <t>CreateArticleWithLongTitleAndWithoutContent</t>
+  </si>
+  <si>
+    <t>NegativeEditArticleWithoutContent</t>
+  </si>
+  <si>
+    <t>TestContent</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Content field is required.</t>
+  </si>
+  <si>
+    <t>NegativeEditArticleWithoutTitle</t>
+  </si>
+  <si>
+    <t>NegativeEditArticleWithLongTitle</t>
+  </si>
+  <si>
+    <t>CreateArticleForNegativeEdit</t>
+  </si>
+  <si>
+    <t>This article is for testing purposes only.</t>
+  </si>
+  <si>
+    <t>NegativeEdit</t>
   </si>
 </sst>
 </file>
@@ -179,12 +282,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -246,7 +350,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -281,7 +385,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -490,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,11 +697,23 @@
       </c>
       <c r="H4" s="1"/>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="3">
+        <v>12345678</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -605,9 +721,252 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Login Logout Tests
Added Login/Logout tests
Added new test sheet in UserData.xls
Moved LoginPage.cs and LoginPageMap.cs in new folder (Pages\LoginLogout)
</commit_message>
<xml_diff>
--- a/Blog-Skeleton/Blog.NUnit.Tests/TestData/UserData.xlsx
+++ b/Blog-Skeleton/Blog.NUnit.Tests/TestData/UserData.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="9105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="9108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginUser" sheetId="1" r:id="rId1"/>
     <sheet name="Articles" sheetId="3" r:id="rId2"/>
-    <sheet name="RegisterUser" sheetId="2" r:id="rId3"/>
+    <sheet name="LoginLogout" sheetId="4" r:id="rId3"/>
+    <sheet name="RegisterUser" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="85">
   <si>
     <t>Key</t>
   </si>
@@ -238,6 +239,39 @@
   </si>
   <si>
     <t>NegativeEdit</t>
+  </si>
+  <si>
+    <t>RememberMeCheck</t>
+  </si>
+  <si>
+    <t>LoginWithRememberMeCheck</t>
+  </si>
+  <si>
+    <t>user1@abv.bg</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>LogoutOfBlog</t>
+  </si>
+  <si>
+    <t>LoginWithAutocomplete</t>
+  </si>
+  <si>
+    <t>LoginWithInvalidEmailAndValidPassword</t>
+  </si>
+  <si>
+    <t>LoginWithValidEmailAndInvalidPassword</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>LoginWithInvalidEmailAndInvalidPassword</t>
+  </si>
+  <si>
+    <t>something</t>
   </si>
 </sst>
 </file>
@@ -600,21 +634,21 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -634,7 +668,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -655,7 +689,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -676,7 +710,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -697,7 +731,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -723,21 +757,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -757,7 +791,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>47</v>
       </c>
@@ -773,7 +807,7 @@
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>50</v>
       </c>
@@ -789,7 +823,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -801,7 +835,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>54</v>
       </c>
@@ -817,7 +851,7 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>57</v>
       </c>
@@ -833,7 +867,7 @@
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>60</v>
       </c>
@@ -851,7 +885,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>61</v>
       </c>
@@ -867,7 +901,7 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>65</v>
       </c>
@@ -885,7 +919,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>71</v>
       </c>
@@ -901,7 +935,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>66</v>
       </c>
@@ -921,7 +955,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>69</v>
       </c>
@@ -939,7 +973,7 @@
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>70</v>
       </c>
@@ -964,23 +998,140 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1000,7 +1151,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1020,7 +1171,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1037,7 +1188,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1054,7 +1205,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1071,7 +1222,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1088,7 +1239,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1108,7 +1259,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1128,7 +1279,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Add LogResultToFileAttribute for ManagePass page
changed name of DB connection of LoginUser to GetTLoginUserData
</commit_message>
<xml_diff>
--- a/Blog-Skeleton/Blog.NUnit.Tests/TestData/UserData.xlsx
+++ b/Blog-Skeleton/Blog.NUnit.Tests/TestData/UserData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="9108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="10905" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="LoginUser" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="85">
   <si>
     <t>Key</t>
   </si>
@@ -142,142 +142,142 @@
     <t>CreateNewArticle</t>
   </si>
   <si>
+    <t>TargetForEdit</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>ArticleErrorMessage</t>
+  </si>
+  <si>
+    <t>AdditionalErrorMessage</t>
+  </si>
+  <si>
+    <t>CreateNewArticleWithValidData</t>
+  </si>
+  <si>
+    <t>TestArticle</t>
+  </si>
+  <si>
+    <t>Dear Reader, this is an article for testing purposes.</t>
+  </si>
+  <si>
+    <t>EditExistingArticle</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>Dear Reader! This is an article for testing purposes!</t>
+  </si>
+  <si>
+    <t>DeleteExistingArticle</t>
+  </si>
+  <si>
+    <t>CreateArticleWithoutTitle</t>
+  </si>
+  <si>
+    <t>The title is empty.</t>
+  </si>
+  <si>
+    <t>The Title field is required.</t>
+  </si>
+  <si>
+    <t>CreateArticleWithoutContent</t>
+  </si>
+  <si>
+    <t>InvalidArticleContent</t>
+  </si>
+  <si>
+    <t>The Content field is required.</t>
+  </si>
+  <si>
+    <t>CreateArticleWithoutTitleAndContent</t>
+  </si>
+  <si>
+    <t>CreateArticleWithLongTitle</t>
+  </si>
+  <si>
+    <t>This article's title is longer than fifty (50) symbols.</t>
+  </si>
+  <si>
+    <t>The title is too long.</t>
+  </si>
+  <si>
+    <t>The field Title must be a string with a maximum length of 50.</t>
+  </si>
+  <si>
+    <t>CreateArticleWithLongTitleAndWithoutContent</t>
+  </si>
+  <si>
+    <t>NegativeEditArticleWithoutContent</t>
+  </si>
+  <si>
+    <t>TestContent</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Content field is required.</t>
+  </si>
+  <si>
+    <t>NegativeEditArticleWithoutTitle</t>
+  </si>
+  <si>
+    <t>NegativeEditArticleWithLongTitle</t>
+  </si>
+  <si>
+    <t>CreateArticleForNegativeEdit</t>
+  </si>
+  <si>
+    <t>This article is for testing purposes only.</t>
+  </si>
+  <si>
+    <t>NegativeEdit</t>
+  </si>
+  <si>
+    <t>RememberMeCheck</t>
+  </si>
+  <si>
+    <t>LoginWithRememberMeCheck</t>
+  </si>
+  <si>
+    <t>user1@abv.bg</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>LogoutOfBlog</t>
+  </si>
+  <si>
+    <t>LoginWithAutocomplete</t>
+  </si>
+  <si>
+    <t>LoginWithInvalidEmailAndValidPassword</t>
+  </si>
+  <si>
+    <t>LoginWithValidEmailAndInvalidPassword</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>LoginWithInvalidEmailAndInvalidPassword</t>
+  </si>
+  <si>
+    <t>something</t>
+  </si>
+  <si>
     <t>abv@abv.bg</t>
-  </si>
-  <si>
-    <t>TargetForEdit</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Content</t>
-  </si>
-  <si>
-    <t>ArticleErrorMessage</t>
-  </si>
-  <si>
-    <t>AdditionalErrorMessage</t>
-  </si>
-  <si>
-    <t>CreateNewArticleWithValidData</t>
-  </si>
-  <si>
-    <t>TestArticle</t>
-  </si>
-  <si>
-    <t>Dear Reader, this is an article for testing purposes.</t>
-  </si>
-  <si>
-    <t>EditExistingArticle</t>
-  </si>
-  <si>
-    <t>Create</t>
-  </si>
-  <si>
-    <t>Dear Reader! This is an article for testing purposes!</t>
-  </si>
-  <si>
-    <t>DeleteExistingArticle</t>
-  </si>
-  <si>
-    <t>CreateArticleWithoutTitle</t>
-  </si>
-  <si>
-    <t>The title is empty.</t>
-  </si>
-  <si>
-    <t>The Title field is required.</t>
-  </si>
-  <si>
-    <t>CreateArticleWithoutContent</t>
-  </si>
-  <si>
-    <t>InvalidArticleContent</t>
-  </si>
-  <si>
-    <t>The Content field is required.</t>
-  </si>
-  <si>
-    <t>CreateArticleWithoutTitleAndContent</t>
-  </si>
-  <si>
-    <t>CreateArticleWithLongTitle</t>
-  </si>
-  <si>
-    <t>This article's title is longer than fifty (50) symbols.</t>
-  </si>
-  <si>
-    <t>The title is too long.</t>
-  </si>
-  <si>
-    <t>The field Title must be a string with a maximum length of 50.</t>
-  </si>
-  <si>
-    <t>CreateArticleWithLongTitleAndWithoutContent</t>
-  </si>
-  <si>
-    <t>NegativeEditArticleWithoutContent</t>
-  </si>
-  <si>
-    <t>TestContent</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The Content field is required.</t>
-  </si>
-  <si>
-    <t>NegativeEditArticleWithoutTitle</t>
-  </si>
-  <si>
-    <t>NegativeEditArticleWithLongTitle</t>
-  </si>
-  <si>
-    <t>CreateArticleForNegativeEdit</t>
-  </si>
-  <si>
-    <t>This article is for testing purposes only.</t>
-  </si>
-  <si>
-    <t>NegativeEdit</t>
-  </si>
-  <si>
-    <t>RememberMeCheck</t>
-  </si>
-  <si>
-    <t>LoginWithRememberMeCheck</t>
-  </si>
-  <si>
-    <t>user1@abv.bg</t>
-  </si>
-  <si>
-    <t>user1</t>
-  </si>
-  <si>
-    <t>LogoutOfBlog</t>
-  </si>
-  <si>
-    <t>LoginWithAutocomplete</t>
-  </si>
-  <si>
-    <t>LoginWithInvalidEmailAndValidPassword</t>
-  </si>
-  <si>
-    <t>LoginWithValidEmailAndInvalidPassword</t>
-  </si>
-  <si>
-    <t>invalid</t>
-  </si>
-  <si>
-    <t>LoginWithInvalidEmailAndInvalidPassword</t>
-  </si>
-  <si>
-    <t>something</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -630,25 +630,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -668,7 +668,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -689,7 +689,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -699,9 +699,6 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
@@ -710,7 +707,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -723,20 +720,17 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
       <c r="F4" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C5" s="3">
         <v>12345678</v>
@@ -761,115 +755,115 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
@@ -882,112 +876,112 @@
         <v>12</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="F13" s="3"/>
     </row>
@@ -1000,17 +994,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1021,88 +1017,88 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>75</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>76</v>
-      </c>
-      <c r="C2" t="s">
-        <v>77</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
         <v>76</v>
-      </c>
-      <c r="C3" t="s">
-        <v>77</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" t="s">
         <v>81</v>
-      </c>
-      <c r="B6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" t="s">
-        <v>82</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" t="s">
         <v>83</v>
       </c>
-      <c r="B7" t="s">
-        <v>84</v>
-      </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
@@ -1121,17 +1117,17 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1151,7 +1147,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1171,7 +1167,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1188,7 +1184,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1205,7 +1201,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1222,7 +1218,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1239,7 +1235,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1259,7 +1255,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1279,7 +1275,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Edit test data for LoginUser
</commit_message>
<xml_diff>
--- a/Blog-Skeleton/Blog.NUnit.Tests/TestData/UserData.xlsx
+++ b/Blog-Skeleton/Blog.NUnit.Tests/TestData/UserData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="10905" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="11505" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="LoginUser" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="85">
   <si>
     <t>Key</t>
   </si>
@@ -631,7 +631,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,6 +699,9 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
@@ -719,6 +722,9 @@
       </c>
       <c r="D4" t="s">
         <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
@@ -752,7 +758,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,7 +1120,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>